<commit_message>
Fixing an improper upright id (numbered 11-20 instead of 1-10).
</commit_message>
<xml_diff>
--- a/Data/phenotypic data/RawData/2011 Data/BogUpper5-R45.xlsx
+++ b/Data/phenotypic data/RawData/2011 Data/BogUpper5-R45.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28125"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="340" windowWidth="11120" windowHeight="8900"/>
+    <workbookView xWindow="480" yWindow="340" windowWidth="18260" windowHeight="14400"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,7 +132,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t xml:space="preserve"> the calyx has 4 flaps of tissue which can be open (strongly folded back), medium, or closed (folded in over calyx)</t>
@@ -146,7 +145,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>these lobes also vary in size, small, medium, large</t>
@@ -160,7 +158,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>rounded, flattened, pointed;  you may also want to note if it is particulary furrowed, or protruding</t>
@@ -174,7 +171,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>rounded, flattened, pointed;  you may also want to note if it is particulary furrowed, or protruding</t>
@@ -188,7 +184,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t xml:space="preserve">each selection has a row/column designation on the plastic bag and has 10 paper bags inside with 1 upright per bag </t>
@@ -211,7 +206,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>measure just this year's growth after flowering, from above the last flower to the tip of the upright.</t>
@@ -232,7 +226,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>these are usually above the fruit and dried remnants of the flower remain</t>
@@ -255,7 +248,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>measure the largest berry per upright</t>
@@ -269,7 +261,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t xml:space="preserve">rate the fruit for amount of bloom, shiny=1, moderate=2, heavy bloom=3 </t>
@@ -290,7 +281,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>- we'll count anything over 5 mm wide as a fruit, this will exclude ovaries that shriveled and didn't develop, check bag for any that fell off in shipping</t>
@@ -304,7 +294,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>measure the largest berry per upright</t>
@@ -318,7 +307,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>weigh all berries</t>
@@ -332,7 +320,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>remove fruit, put upright back in paper bag and dry sample in oven. Once dry, leaves will fall off easily. You may want to keep bags in order, staple them together, and label 1st bag with row/col designation, then put in oven</t>
@@ -346,7 +333,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>weigh the berry you measured</t>
@@ -360,7 +346,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>see figures, round, oval (an elongated round), oblong (elongated round with squared ends), pyriform (pear-shaped), spindle (elongated with both ends pointy, I doubt you will have any of these)</t>
@@ -383,7 +368,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t xml:space="preserve"> count developed seeds in the largest berry (developed seeds are approx 1.5mm long x 1.5mm wide, you will also find smaller, softer and usually lighter in color undeveloped seeds, don't count these)</t>
@@ -404,7 +388,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>- with these pedicels, fruit was probably set and then developed and fell off or rotted early on and fell off, sometimes you will also find aborted flowers below the set fruit)</t>
@@ -903,10 +886,6 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -921,6 +900,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1256,8 +1239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W404"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D31" workbookViewId="0">
-      <selection activeCell="N31" sqref="A1:T1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A89" sqref="A89:A98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -1330,53 +1313,53 @@
       <c r="U2" s="17"/>
     </row>
     <row r="3" spans="1:21" ht="32.25" customHeight="1">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
-      <c r="L3" s="67"/>
-      <c r="M3" s="67"/>
-      <c r="N3" s="67"/>
-      <c r="O3" s="67"/>
-      <c r="P3" s="67"/>
-      <c r="Q3" s="67"/>
-      <c r="R3" s="67"/>
-      <c r="S3" s="67"/>
-      <c r="T3" s="67"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="66"/>
+      <c r="Q3" s="66"/>
+      <c r="R3" s="66"/>
+      <c r="S3" s="66"/>
+      <c r="T3" s="66"/>
       <c r="U3" s="38"/>
     </row>
     <row r="4" spans="1:21" ht="30.75" customHeight="1">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="66" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
-      <c r="L4" s="67"/>
-      <c r="M4" s="67"/>
-      <c r="N4" s="67"/>
-      <c r="O4" s="67"/>
-      <c r="P4" s="67"/>
-      <c r="Q4" s="67"/>
-      <c r="R4" s="67"/>
-      <c r="S4" s="67"/>
-      <c r="T4" s="67"/>
+      <c r="B4" s="66"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="66"/>
+      <c r="J4" s="66"/>
+      <c r="K4" s="66"/>
+      <c r="L4" s="66"/>
+      <c r="M4" s="66"/>
+      <c r="N4" s="66"/>
+      <c r="O4" s="66"/>
+      <c r="P4" s="66"/>
+      <c r="Q4" s="66"/>
+      <c r="R4" s="66"/>
+      <c r="S4" s="66"/>
+      <c r="T4" s="66"/>
       <c r="U4" s="38"/>
     </row>
     <row r="5" spans="1:21" ht="19.5" customHeight="1">
@@ -1488,28 +1471,28 @@
       <c r="U9" s="17"/>
     </row>
     <row r="10" spans="1:21" ht="30.75" customHeight="1">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="66"/>
-      <c r="E10" s="66"/>
-      <c r="F10" s="66"/>
-      <c r="G10" s="66"/>
-      <c r="H10" s="66"/>
-      <c r="I10" s="66"/>
-      <c r="J10" s="66"/>
-      <c r="K10" s="66"/>
-      <c r="L10" s="66"/>
-      <c r="M10" s="66"/>
-      <c r="N10" s="66"/>
-      <c r="O10" s="66"/>
-      <c r="P10" s="66"/>
-      <c r="Q10" s="66"/>
-      <c r="R10" s="66"/>
-      <c r="S10" s="66"/>
-      <c r="T10" s="66"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="65"/>
+      <c r="E10" s="65"/>
+      <c r="F10" s="65"/>
+      <c r="G10" s="65"/>
+      <c r="H10" s="65"/>
+      <c r="I10" s="65"/>
+      <c r="J10" s="65"/>
+      <c r="K10" s="65"/>
+      <c r="L10" s="65"/>
+      <c r="M10" s="65"/>
+      <c r="N10" s="65"/>
+      <c r="O10" s="65"/>
+      <c r="P10" s="65"/>
+      <c r="Q10" s="65"/>
+      <c r="R10" s="65"/>
+      <c r="S10" s="65"/>
+      <c r="T10" s="65"/>
       <c r="U10" s="32"/>
     </row>
     <row r="11" spans="1:21" ht="16.5" customHeight="1">
@@ -1682,78 +1665,78 @@
       <c r="B19" s="9"/>
     </row>
     <row r="20" spans="1:22" ht="18.75" customHeight="1">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="65" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="66"/>
-      <c r="C20" s="66"/>
-      <c r="D20" s="66"/>
-      <c r="E20" s="66"/>
-      <c r="F20" s="66"/>
-      <c r="G20" s="66"/>
-      <c r="H20" s="66"/>
-      <c r="I20" s="66"/>
-      <c r="J20" s="66"/>
-      <c r="K20" s="66"/>
-      <c r="L20" s="66"/>
-      <c r="M20" s="66"/>
-      <c r="N20" s="66"/>
-      <c r="O20" s="66"/>
-      <c r="P20" s="66"/>
-      <c r="Q20" s="66"/>
-      <c r="R20" s="66"/>
-      <c r="S20" s="66"/>
-      <c r="T20" s="66"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="65"/>
+      <c r="D20" s="65"/>
+      <c r="E20" s="65"/>
+      <c r="F20" s="65"/>
+      <c r="G20" s="65"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
+      <c r="K20" s="65"/>
+      <c r="L20" s="65"/>
+      <c r="M20" s="65"/>
+      <c r="N20" s="65"/>
+      <c r="O20" s="65"/>
+      <c r="P20" s="65"/>
+      <c r="Q20" s="65"/>
+      <c r="R20" s="65"/>
+      <c r="S20" s="65"/>
+      <c r="T20" s="65"/>
       <c r="U20" s="32"/>
     </row>
     <row r="21" spans="1:22" ht="27.75" customHeight="1">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="66"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="66"/>
-      <c r="E21" s="66"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="66"/>
-      <c r="H21" s="66"/>
-      <c r="I21" s="66"/>
-      <c r="J21" s="66"/>
-      <c r="K21" s="66"/>
-      <c r="L21" s="66"/>
-      <c r="M21" s="66"/>
-      <c r="N21" s="66"/>
-      <c r="O21" s="66"/>
-      <c r="P21" s="66"/>
-      <c r="Q21" s="66"/>
-      <c r="R21" s="66"/>
-      <c r="S21" s="66"/>
-      <c r="T21" s="66"/>
+      <c r="B21" s="65"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="65"/>
+      <c r="F21" s="65"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
+      <c r="K21" s="65"/>
+      <c r="L21" s="65"/>
+      <c r="M21" s="65"/>
+      <c r="N21" s="65"/>
+      <c r="O21" s="65"/>
+      <c r="P21" s="65"/>
+      <c r="Q21" s="65"/>
+      <c r="R21" s="65"/>
+      <c r="S21" s="65"/>
+      <c r="T21" s="65"/>
       <c r="U21" s="32"/>
     </row>
     <row r="22" spans="1:22" ht="33" customHeight="1">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="65" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="66"/>
-      <c r="C22" s="66"/>
-      <c r="D22" s="66"/>
-      <c r="E22" s="66"/>
-      <c r="F22" s="66"/>
-      <c r="G22" s="66"/>
-      <c r="H22" s="66"/>
-      <c r="I22" s="66"/>
-      <c r="J22" s="66"/>
-      <c r="K22" s="66"/>
-      <c r="L22" s="66"/>
-      <c r="M22" s="66"/>
-      <c r="N22" s="66"/>
-      <c r="O22" s="66"/>
-      <c r="P22" s="66"/>
-      <c r="Q22" s="66"/>
-      <c r="R22" s="66"/>
-      <c r="S22" s="66"/>
-      <c r="T22" s="66"/>
+      <c r="B22" s="65"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="65"/>
+      <c r="K22" s="65"/>
+      <c r="L22" s="65"/>
+      <c r="M22" s="65"/>
+      <c r="N22" s="65"/>
+      <c r="O22" s="65"/>
+      <c r="P22" s="65"/>
+      <c r="Q22" s="65"/>
+      <c r="R22" s="65"/>
+      <c r="S22" s="65"/>
+      <c r="T22" s="65"/>
       <c r="U22" s="32"/>
     </row>
     <row r="24" spans="1:22" ht="19.5" customHeight="1">
@@ -1824,10 +1807,10 @@
       <c r="L32" s="21"/>
       <c r="M32" s="17"/>
       <c r="N32" s="55"/>
-      <c r="O32" s="65" t="s">
+      <c r="O32" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="P32" s="65"/>
+      <c r="P32" s="64"/>
       <c r="Q32" s="5"/>
       <c r="T32" s="3"/>
       <c r="V32" s="17"/>
@@ -1842,11 +1825,11 @@
         <v>16</v>
       </c>
       <c r="J33" s="24"/>
-      <c r="K33" s="64" t="s">
+      <c r="K33" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="L33" s="64"/>
-      <c r="M33" s="64"/>
+      <c r="L33" s="63"/>
+      <c r="M33" s="63"/>
       <c r="N33" s="59" t="s">
         <v>23</v>
       </c>
@@ -3398,11 +3381,11 @@
         <v>16</v>
       </c>
       <c r="J59" s="24"/>
-      <c r="K59" s="64" t="s">
+      <c r="K59" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="L59" s="64"/>
-      <c r="M59" s="64"/>
+      <c r="L59" s="63"/>
+      <c r="M59" s="63"/>
       <c r="N59" s="59" t="s">
         <v>23</v>
       </c>
@@ -4269,7 +4252,7 @@
     </row>
     <row r="75" spans="1:22" ht="19.5" customHeight="1">
       <c r="A75" s="4">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B75" s="3">
         <v>5</v>
@@ -4331,7 +4314,7 @@
     </row>
     <row r="76" spans="1:22" ht="19.5" customHeight="1">
       <c r="A76" s="4">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B76" s="3">
         <v>2</v>
@@ -4397,7 +4380,7 @@
     </row>
     <row r="77" spans="1:22" ht="19.5" customHeight="1">
       <c r="A77" s="4">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B77" s="3">
         <v>5</v>
@@ -4463,7 +4446,7 @@
     </row>
     <row r="78" spans="1:22" ht="19.5" customHeight="1">
       <c r="A78" s="4">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B78" s="3">
         <v>3</v>
@@ -4528,7 +4511,7 @@
     </row>
     <row r="79" spans="1:22" ht="19.5" customHeight="1">
       <c r="A79" s="4">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B79" s="3">
         <v>5</v>
@@ -4593,7 +4576,7 @@
     </row>
     <row r="80" spans="1:22" ht="19.5" customHeight="1">
       <c r="A80" s="4">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B80" s="3">
         <v>4</v>
@@ -4661,7 +4644,7 @@
     </row>
     <row r="81" spans="1:22" ht="19.5" customHeight="1">
       <c r="A81" s="4">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B81" s="3">
         <v>5</v>
@@ -4726,7 +4709,7 @@
     </row>
     <row r="82" spans="1:22" ht="19.5" customHeight="1">
       <c r="A82" s="4">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B82" s="3">
         <v>2</v>
@@ -4791,7 +4774,7 @@
     </row>
     <row r="83" spans="1:22" ht="19.5" customHeight="1">
       <c r="A83" s="4">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B83" s="3">
         <v>3</v>
@@ -4856,7 +4839,7 @@
     </row>
     <row r="84" spans="1:22" ht="19.5" customHeight="1">
       <c r="A84" s="4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B84" s="3">
         <v>2</v>
@@ -4929,11 +4912,11 @@
         <v>16</v>
       </c>
       <c r="J85" s="24"/>
-      <c r="K85" s="64" t="s">
+      <c r="K85" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="L85" s="64"/>
-      <c r="M85" s="64"/>
+      <c r="L85" s="63"/>
+      <c r="M85" s="63"/>
       <c r="N85" s="59" t="s">
         <v>23</v>
       </c>
@@ -5110,7 +5093,7 @@
     </row>
     <row r="89" spans="1:22" ht="19.5" customHeight="1">
       <c r="A89" s="4">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B89" s="3">
         <v>5</v>
@@ -5175,7 +5158,7 @@
     </row>
     <row r="90" spans="1:22" ht="19.5" customHeight="1">
       <c r="A90" s="4">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="B90" s="3">
         <v>4</v>
@@ -5241,7 +5224,7 @@
     </row>
     <row r="91" spans="1:22" ht="19.5" customHeight="1">
       <c r="A91" s="4">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B91" s="3">
         <v>5</v>
@@ -5307,7 +5290,7 @@
     </row>
     <row r="92" spans="1:22" ht="19.5" customHeight="1">
       <c r="A92" s="4">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="B92" s="3">
         <v>5</v>
@@ -5372,7 +5355,7 @@
     </row>
     <row r="93" spans="1:22" ht="19.5" customHeight="1">
       <c r="A93" s="4">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="B93" s="3">
         <v>5</v>
@@ -5437,7 +5420,7 @@
     </row>
     <row r="94" spans="1:22" ht="19.5" customHeight="1">
       <c r="A94" s="4">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B94" s="3">
         <v>2</v>
@@ -5502,7 +5485,7 @@
     </row>
     <row r="95" spans="1:22" ht="19.5" customHeight="1">
       <c r="A95" s="4">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="B95" s="3">
         <v>4</v>
@@ -5568,7 +5551,7 @@
     </row>
     <row r="96" spans="1:22" ht="19.5" customHeight="1">
       <c r="A96" s="4">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B96" s="3">
         <v>6</v>
@@ -5633,7 +5616,7 @@
     </row>
     <row r="97" spans="1:22" ht="19.5" customHeight="1">
       <c r="A97" s="4">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B97" s="3">
         <v>4</v>
@@ -5698,7 +5681,7 @@
     </row>
     <row r="98" spans="1:22" ht="19.5" customHeight="1">
       <c r="A98" s="4">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B98" s="3">
         <v>7</v>
@@ -6042,9 +6025,9 @@
       <c r="H111" s="49"/>
       <c r="I111" s="26"/>
       <c r="J111" s="50"/>
-      <c r="K111" s="63"/>
-      <c r="L111" s="63"/>
-      <c r="M111" s="63"/>
+      <c r="K111" s="67"/>
+      <c r="L111" s="67"/>
+      <c r="M111" s="67"/>
       <c r="N111" s="62"/>
       <c r="O111" s="51"/>
       <c r="P111" s="26"/>
@@ -6666,9 +6649,9 @@
       <c r="H137" s="49"/>
       <c r="I137" s="26"/>
       <c r="J137" s="50"/>
-      <c r="K137" s="63"/>
-      <c r="L137" s="63"/>
-      <c r="M137" s="63"/>
+      <c r="K137" s="67"/>
+      <c r="L137" s="67"/>
+      <c r="M137" s="67"/>
       <c r="N137" s="62"/>
       <c r="O137" s="51"/>
       <c r="P137" s="26"/>
@@ -7290,9 +7273,9 @@
       <c r="H163" s="49"/>
       <c r="I163" s="26"/>
       <c r="J163" s="50"/>
-      <c r="K163" s="63"/>
-      <c r="L163" s="63"/>
-      <c r="M163" s="63"/>
+      <c r="K163" s="67"/>
+      <c r="L163" s="67"/>
+      <c r="M163" s="67"/>
       <c r="N163" s="62"/>
       <c r="O163" s="51"/>
       <c r="P163" s="26"/>
@@ -7914,9 +7897,9 @@
       <c r="H189" s="49"/>
       <c r="I189" s="26"/>
       <c r="J189" s="50"/>
-      <c r="K189" s="63"/>
-      <c r="L189" s="63"/>
-      <c r="M189" s="63"/>
+      <c r="K189" s="67"/>
+      <c r="L189" s="67"/>
+      <c r="M189" s="67"/>
       <c r="N189" s="62"/>
       <c r="O189" s="51"/>
       <c r="P189" s="26"/>
@@ -8538,9 +8521,9 @@
       <c r="H215" s="49"/>
       <c r="I215" s="26"/>
       <c r="J215" s="50"/>
-      <c r="K215" s="63"/>
-      <c r="L215" s="63"/>
-      <c r="M215" s="63"/>
+      <c r="K215" s="67"/>
+      <c r="L215" s="67"/>
+      <c r="M215" s="67"/>
       <c r="N215" s="62"/>
       <c r="O215" s="51"/>
       <c r="P215" s="26"/>
@@ -13089,6 +13072,13 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="K215:M215"/>
+    <mergeCell ref="K59:M59"/>
+    <mergeCell ref="K85:M85"/>
+    <mergeCell ref="K111:M111"/>
+    <mergeCell ref="K137:M137"/>
+    <mergeCell ref="K163:M163"/>
+    <mergeCell ref="K189:M189"/>
     <mergeCell ref="K33:M33"/>
     <mergeCell ref="O32:P32"/>
     <mergeCell ref="A22:T22"/>
@@ -13097,13 +13087,6 @@
     <mergeCell ref="A20:T20"/>
     <mergeCell ref="A21:T21"/>
     <mergeCell ref="A10:T10"/>
-    <mergeCell ref="K215:M215"/>
-    <mergeCell ref="K59:M59"/>
-    <mergeCell ref="K85:M85"/>
-    <mergeCell ref="K111:M111"/>
-    <mergeCell ref="K137:M137"/>
-    <mergeCell ref="K163:M163"/>
-    <mergeCell ref="K189:M189"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions gridLines="1"/>

</xml_diff>

<commit_message>
Fixing mislabeled upright identifiers
</commit_message>
<xml_diff>
--- a/Data/phenotypic data/RawData/2011 Data/BogUpper5-R45.xlsx
+++ b/Data/phenotypic data/RawData/2011 Data/BogUpper5-R45.xlsx
@@ -132,7 +132,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t xml:space="preserve"> the calyx has 4 flaps of tissue which can be open (strongly folded back), medium, or closed (folded in over calyx)</t>
@@ -146,7 +145,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>these lobes also vary in size, small, medium, large</t>
@@ -160,7 +158,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>rounded, flattened, pointed;  you may also want to note if it is particulary furrowed, or protruding</t>
@@ -174,7 +171,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>rounded, flattened, pointed;  you may also want to note if it is particulary furrowed, or protruding</t>
@@ -188,7 +184,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t xml:space="preserve">each selection has a row/column designation on the plastic bag and has 10 paper bags inside with 1 upright per bag </t>
@@ -211,7 +206,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>measure just this year's growth after flowering, from above the last flower to the tip of the upright.</t>
@@ -232,7 +226,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>these are usually above the fruit and dried remnants of the flower remain</t>
@@ -255,7 +248,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>measure the largest berry per upright</t>
@@ -269,7 +261,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t xml:space="preserve">rate the fruit for amount of bloom, shiny=1, moderate=2, heavy bloom=3 </t>
@@ -290,7 +281,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>- we'll count anything over 5 mm wide as a fruit, this will exclude ovaries that shriveled and didn't develop, check bag for any that fell off in shipping</t>
@@ -304,7 +294,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>measure the largest berry per upright</t>
@@ -318,7 +307,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>weigh all berries</t>
@@ -332,7 +320,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>remove fruit, put upright back in paper bag and dry sample in oven. Once dry, leaves will fall off easily. You may want to keep bags in order, staple them together, and label 1st bag with row/col designation, then put in oven</t>
@@ -346,7 +333,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>weigh the berry you measured</t>
@@ -360,7 +346,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>see figures, round, oval (an elongated round), oblong (elongated round with squared ends), pyriform (pear-shaped), spindle (elongated with both ends pointy, I doubt you will have any of these)</t>
@@ -383,7 +368,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t xml:space="preserve"> count developed seeds in the largest berry (developed seeds are approx 1.5mm long x 1.5mm wide, you will also find smaller, softer and usually lighter in color undeveloped seeds, don't count these)</t>
@@ -404,7 +388,6 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
-        <family val="2"/>
         <charset val="204"/>
       </rPr>
       <t>- with these pedicels, fruit was probably set and then developed and fell off or rotted early on and fell off, sometimes you will also find aborted flowers below the set fruit)</t>
@@ -894,6 +877,10 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
@@ -908,10 +895,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1247,8 +1230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W404"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="V92" sqref="V92"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A94" sqref="A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0"/>
@@ -1323,53 +1306,53 @@
       <c r="U2" s="17"/>
     </row>
     <row r="3" spans="1:21" ht="32.25" customHeight="1">
-      <c r="A3" s="66" t="s">
+      <c r="A3" s="67" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
-      <c r="M3" s="66"/>
-      <c r="N3" s="66"/>
-      <c r="O3" s="66"/>
-      <c r="P3" s="66"/>
-      <c r="Q3" s="66"/>
-      <c r="R3" s="66"/>
-      <c r="S3" s="66"/>
-      <c r="T3" s="66"/>
+      <c r="B3" s="67"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="67"/>
+      <c r="P3" s="67"/>
+      <c r="Q3" s="67"/>
+      <c r="R3" s="67"/>
+      <c r="S3" s="67"/>
+      <c r="T3" s="67"/>
       <c r="U3" s="38"/>
     </row>
     <row r="4" spans="1:21" ht="30.75" customHeight="1">
-      <c r="A4" s="66" t="s">
+      <c r="A4" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="66"/>
-      <c r="C4" s="66"/>
-      <c r="D4" s="66"/>
-      <c r="E4" s="66"/>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
-      <c r="O4" s="66"/>
-      <c r="P4" s="66"/>
-      <c r="Q4" s="66"/>
-      <c r="R4" s="66"/>
-      <c r="S4" s="66"/>
-      <c r="T4" s="66"/>
+      <c r="B4" s="67"/>
+      <c r="C4" s="67"/>
+      <c r="D4" s="67"/>
+      <c r="E4" s="67"/>
+      <c r="F4" s="67"/>
+      <c r="G4" s="67"/>
+      <c r="H4" s="67"/>
+      <c r="I4" s="67"/>
+      <c r="J4" s="67"/>
+      <c r="K4" s="67"/>
+      <c r="L4" s="67"/>
+      <c r="M4" s="67"/>
+      <c r="N4" s="67"/>
+      <c r="O4" s="67"/>
+      <c r="P4" s="67"/>
+      <c r="Q4" s="67"/>
+      <c r="R4" s="67"/>
+      <c r="S4" s="67"/>
+      <c r="T4" s="67"/>
       <c r="U4" s="38"/>
     </row>
     <row r="5" spans="1:21" ht="19.5" customHeight="1">
@@ -1481,28 +1464,28 @@
       <c r="U9" s="17"/>
     </row>
     <row r="10" spans="1:21" ht="30.75" customHeight="1">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="B10" s="65"/>
-      <c r="C10" s="65"/>
-      <c r="D10" s="65"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="65"/>
-      <c r="G10" s="65"/>
-      <c r="H10" s="65"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="65"/>
-      <c r="K10" s="65"/>
-      <c r="L10" s="65"/>
-      <c r="M10" s="65"/>
-      <c r="N10" s="65"/>
-      <c r="O10" s="65"/>
-      <c r="P10" s="65"/>
-      <c r="Q10" s="65"/>
-      <c r="R10" s="65"/>
-      <c r="S10" s="65"/>
-      <c r="T10" s="65"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="66"/>
+      <c r="K10" s="66"/>
+      <c r="L10" s="66"/>
+      <c r="M10" s="66"/>
+      <c r="N10" s="66"/>
+      <c r="O10" s="66"/>
+      <c r="P10" s="66"/>
+      <c r="Q10" s="66"/>
+      <c r="R10" s="66"/>
+      <c r="S10" s="66"/>
+      <c r="T10" s="66"/>
       <c r="U10" s="32"/>
     </row>
     <row r="11" spans="1:21" ht="16.5" customHeight="1">
@@ -1675,78 +1658,78 @@
       <c r="B19" s="9"/>
     </row>
     <row r="20" spans="1:22" ht="18.75" customHeight="1">
-      <c r="A20" s="65" t="s">
+      <c r="A20" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="65"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="65"/>
-      <c r="G20" s="65"/>
-      <c r="H20" s="65"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="65"/>
-      <c r="K20" s="65"/>
-      <c r="L20" s="65"/>
-      <c r="M20" s="65"/>
-      <c r="N20" s="65"/>
-      <c r="O20" s="65"/>
-      <c r="P20" s="65"/>
-      <c r="Q20" s="65"/>
-      <c r="R20" s="65"/>
-      <c r="S20" s="65"/>
-      <c r="T20" s="65"/>
+      <c r="B20" s="66"/>
+      <c r="C20" s="66"/>
+      <c r="D20" s="66"/>
+      <c r="E20" s="66"/>
+      <c r="F20" s="66"/>
+      <c r="G20" s="66"/>
+      <c r="H20" s="66"/>
+      <c r="I20" s="66"/>
+      <c r="J20" s="66"/>
+      <c r="K20" s="66"/>
+      <c r="L20" s="66"/>
+      <c r="M20" s="66"/>
+      <c r="N20" s="66"/>
+      <c r="O20" s="66"/>
+      <c r="P20" s="66"/>
+      <c r="Q20" s="66"/>
+      <c r="R20" s="66"/>
+      <c r="S20" s="66"/>
+      <c r="T20" s="66"/>
       <c r="U20" s="32"/>
     </row>
     <row r="21" spans="1:22" ht="27.75" customHeight="1">
-      <c r="A21" s="65" t="s">
+      <c r="A21" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="B21" s="65"/>
-      <c r="C21" s="65"/>
-      <c r="D21" s="65"/>
-      <c r="E21" s="65"/>
-      <c r="F21" s="65"/>
-      <c r="G21" s="65"/>
-      <c r="H21" s="65"/>
-      <c r="I21" s="65"/>
-      <c r="J21" s="65"/>
-      <c r="K21" s="65"/>
-      <c r="L21" s="65"/>
-      <c r="M21" s="65"/>
-      <c r="N21" s="65"/>
-      <c r="O21" s="65"/>
-      <c r="P21" s="65"/>
-      <c r="Q21" s="65"/>
-      <c r="R21" s="65"/>
-      <c r="S21" s="65"/>
-      <c r="T21" s="65"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="66"/>
+      <c r="D21" s="66"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="66"/>
+      <c r="G21" s="66"/>
+      <c r="H21" s="66"/>
+      <c r="I21" s="66"/>
+      <c r="J21" s="66"/>
+      <c r="K21" s="66"/>
+      <c r="L21" s="66"/>
+      <c r="M21" s="66"/>
+      <c r="N21" s="66"/>
+      <c r="O21" s="66"/>
+      <c r="P21" s="66"/>
+      <c r="Q21" s="66"/>
+      <c r="R21" s="66"/>
+      <c r="S21" s="66"/>
+      <c r="T21" s="66"/>
       <c r="U21" s="32"/>
     </row>
     <row r="22" spans="1:22" ht="33" customHeight="1">
-      <c r="A22" s="65" t="s">
+      <c r="A22" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="65"/>
-      <c r="C22" s="65"/>
-      <c r="D22" s="65"/>
-      <c r="E22" s="65"/>
-      <c r="F22" s="65"/>
-      <c r="G22" s="65"/>
-      <c r="H22" s="65"/>
-      <c r="I22" s="65"/>
-      <c r="J22" s="65"/>
-      <c r="K22" s="65"/>
-      <c r="L22" s="65"/>
-      <c r="M22" s="65"/>
-      <c r="N22" s="65"/>
-      <c r="O22" s="65"/>
-      <c r="P22" s="65"/>
-      <c r="Q22" s="65"/>
-      <c r="R22" s="65"/>
-      <c r="S22" s="65"/>
-      <c r="T22" s="65"/>
+      <c r="B22" s="66"/>
+      <c r="C22" s="66"/>
+      <c r="D22" s="66"/>
+      <c r="E22" s="66"/>
+      <c r="F22" s="66"/>
+      <c r="G22" s="66"/>
+      <c r="H22" s="66"/>
+      <c r="I22" s="66"/>
+      <c r="J22" s="66"/>
+      <c r="K22" s="66"/>
+      <c r="L22" s="66"/>
+      <c r="M22" s="66"/>
+      <c r="N22" s="66"/>
+      <c r="O22" s="66"/>
+      <c r="P22" s="66"/>
+      <c r="Q22" s="66"/>
+      <c r="R22" s="66"/>
+      <c r="S22" s="66"/>
+      <c r="T22" s="66"/>
       <c r="U22" s="32"/>
     </row>
     <row r="24" spans="1:22" ht="19.5" customHeight="1">
@@ -1817,10 +1800,10 @@
       <c r="L32" s="21"/>
       <c r="M32" s="17"/>
       <c r="N32" s="55"/>
-      <c r="O32" s="64" t="s">
+      <c r="O32" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="P32" s="64"/>
+      <c r="P32" s="65"/>
       <c r="Q32" s="5"/>
       <c r="T32" s="3"/>
       <c r="V32" s="17"/>
@@ -1835,11 +1818,11 @@
         <v>16</v>
       </c>
       <c r="J33" s="24"/>
-      <c r="K33" s="63" t="s">
+      <c r="K33" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="L33" s="63"/>
-      <c r="M33" s="63"/>
+      <c r="L33" s="64"/>
+      <c r="M33" s="64"/>
       <c r="N33" s="59" t="s">
         <v>23</v>
       </c>
@@ -3388,11 +3371,11 @@
         <v>16</v>
       </c>
       <c r="J59" s="24"/>
-      <c r="K59" s="63" t="s">
+      <c r="K59" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="L59" s="63"/>
-      <c r="M59" s="63"/>
+      <c r="L59" s="64"/>
+      <c r="M59" s="64"/>
       <c r="N59" s="59" t="s">
         <v>23</v>
       </c>
@@ -4919,11 +4902,11 @@
         <v>16</v>
       </c>
       <c r="J85" s="24"/>
-      <c r="K85" s="63" t="s">
+      <c r="K85" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="L85" s="63"/>
-      <c r="M85" s="63"/>
+      <c r="L85" s="64"/>
+      <c r="M85" s="64"/>
       <c r="N85" s="59" t="s">
         <v>23</v>
       </c>
@@ -5297,7 +5280,7 @@
     </row>
     <row r="92" spans="1:22" ht="19.5" customHeight="1">
       <c r="A92" s="4">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B92" s="3">
         <v>5</v>
@@ -5362,7 +5345,7 @@
     </row>
     <row r="93" spans="1:22" ht="19.5" customHeight="1">
       <c r="A93" s="4">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B93" s="3">
         <v>5</v>
@@ -6032,9 +6015,9 @@
       <c r="H111" s="49"/>
       <c r="I111" s="26"/>
       <c r="J111" s="50"/>
-      <c r="K111" s="67"/>
-      <c r="L111" s="67"/>
-      <c r="M111" s="67"/>
+      <c r="K111" s="63"/>
+      <c r="L111" s="63"/>
+      <c r="M111" s="63"/>
       <c r="N111" s="62"/>
       <c r="O111" s="51"/>
       <c r="P111" s="26"/>
@@ -6656,9 +6639,9 @@
       <c r="H137" s="49"/>
       <c r="I137" s="26"/>
       <c r="J137" s="50"/>
-      <c r="K137" s="67"/>
-      <c r="L137" s="67"/>
-      <c r="M137" s="67"/>
+      <c r="K137" s="63"/>
+      <c r="L137" s="63"/>
+      <c r="M137" s="63"/>
       <c r="N137" s="62"/>
       <c r="O137" s="51"/>
       <c r="P137" s="26"/>
@@ -7280,9 +7263,9 @@
       <c r="H163" s="49"/>
       <c r="I163" s="26"/>
       <c r="J163" s="50"/>
-      <c r="K163" s="67"/>
-      <c r="L163" s="67"/>
-      <c r="M163" s="67"/>
+      <c r="K163" s="63"/>
+      <c r="L163" s="63"/>
+      <c r="M163" s="63"/>
       <c r="N163" s="62"/>
       <c r="O163" s="51"/>
       <c r="P163" s="26"/>
@@ -7904,9 +7887,9 @@
       <c r="H189" s="49"/>
       <c r="I189" s="26"/>
       <c r="J189" s="50"/>
-      <c r="K189" s="67"/>
-      <c r="L189" s="67"/>
-      <c r="M189" s="67"/>
+      <c r="K189" s="63"/>
+      <c r="L189" s="63"/>
+      <c r="M189" s="63"/>
       <c r="N189" s="62"/>
       <c r="O189" s="51"/>
       <c r="P189" s="26"/>
@@ -8528,9 +8511,9 @@
       <c r="H215" s="49"/>
       <c r="I215" s="26"/>
       <c r="J215" s="50"/>
-      <c r="K215" s="67"/>
-      <c r="L215" s="67"/>
-      <c r="M215" s="67"/>
+      <c r="K215" s="63"/>
+      <c r="L215" s="63"/>
+      <c r="M215" s="63"/>
       <c r="N215" s="62"/>
       <c r="O215" s="51"/>
       <c r="P215" s="26"/>
@@ -13079,13 +13062,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="K215:M215"/>
-    <mergeCell ref="K59:M59"/>
-    <mergeCell ref="K85:M85"/>
-    <mergeCell ref="K111:M111"/>
-    <mergeCell ref="K137:M137"/>
-    <mergeCell ref="K163:M163"/>
-    <mergeCell ref="K189:M189"/>
     <mergeCell ref="K33:M33"/>
     <mergeCell ref="O32:P32"/>
     <mergeCell ref="A22:T22"/>
@@ -13094,6 +13070,13 @@
     <mergeCell ref="A20:T20"/>
     <mergeCell ref="A21:T21"/>
     <mergeCell ref="A10:T10"/>
+    <mergeCell ref="K215:M215"/>
+    <mergeCell ref="K59:M59"/>
+    <mergeCell ref="K85:M85"/>
+    <mergeCell ref="K111:M111"/>
+    <mergeCell ref="K137:M137"/>
+    <mergeCell ref="K163:M163"/>
+    <mergeCell ref="K189:M189"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions gridLines="1"/>

</xml_diff>